<commit_message>
Add Excel files mapping for the Reservation entity
</commit_message>
<xml_diff>
--- a/RoomOccupancy.Persistence/Initializer/Files/SaleWzim.xlsx
+++ b/RoomOccupancy.Persistence/Initializer/Files/SaleWzim.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
   <si>
     <t xml:space="preserve"> Aula IV </t>
   </si>
@@ -50,15 +50,6 @@
   </si>
   <si>
     <t>Budynek</t>
-  </si>
-  <si>
-    <t>nazwa</t>
-  </si>
-  <si>
-    <t>projekt</t>
-  </si>
-  <si>
-    <t>powierzchnia</t>
   </si>
 </sst>
 </file>
@@ -468,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,10 +473,9 @@
     <col min="4" max="4" width="23.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -504,17 +494,8 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>34</v>
       </c>
@@ -534,7 +515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>34</v>
       </c>
@@ -554,7 +535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>34</v>
       </c>
@@ -574,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>34</v>
       </c>
@@ -594,7 +575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>34</v>
       </c>
@@ -614,7 +595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>34</v>
       </c>
@@ -634,7 +615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>34</v>
       </c>
@@ -654,7 +635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>34</v>
       </c>
@@ -674,7 +655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>34</v>
       </c>
@@ -694,7 +675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>34</v>
       </c>
@@ -714,7 +695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>34</v>
       </c>
@@ -734,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>34</v>
       </c>
@@ -754,7 +735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>34</v>
       </c>
@@ -774,7 +755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>34</v>
       </c>
@@ -794,7 +775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Update Equipment entity seeding files.
</commit_message>
<xml_diff>
--- a/RoomOccupancy.Persistence/Initializer/Files/SaleWzim.xlsx
+++ b/RoomOccupancy.Persistence/Initializer/Files/SaleWzim.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
   <si>
     <t xml:space="preserve"> Aula IV </t>
   </si>
@@ -50,6 +50,30 @@
   </si>
   <si>
     <t>Budynek</t>
+  </si>
+  <si>
+    <t>Wyposażenie</t>
+  </si>
+  <si>
+    <t>Projektor</t>
+  </si>
+  <si>
+    <t>laboratorium komputerowe</t>
+  </si>
+  <si>
+    <t>Urządzenia sieciowe i budowa sieci, Projektor</t>
+  </si>
+  <si>
+    <t>Oscyloskop, Płytka badawcza układu scalonego</t>
+  </si>
+  <si>
+    <t>Projektor, Stanowiska komputerowe</t>
+  </si>
+  <si>
+    <t>Stanowiska komputerowe, Urządzenia sieciowe i budowa sieci, Projektor</t>
+  </si>
+  <si>
+    <t>Płytka badawcza układu scalonego, Oscyloskop</t>
   </si>
 </sst>
 </file>
@@ -459,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,9 +497,10 @@
     <col min="4" max="4" width="23.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -494,8 +519,11 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>34</v>
       </c>
@@ -514,8 +542,11 @@
       <c r="F2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>34</v>
       </c>
@@ -534,8 +565,11 @@
       <c r="F3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>34</v>
       </c>
@@ -555,7 +589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>34</v>
       </c>
@@ -574,8 +608,11 @@
       <c r="F5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>34</v>
       </c>
@@ -594,8 +631,11 @@
       <c r="F6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>34</v>
       </c>
@@ -614,8 +654,11 @@
       <c r="F7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>34</v>
       </c>
@@ -629,13 +672,16 @@
         <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>34</v>
       </c>
@@ -654,8 +700,11 @@
       <c r="F9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>34</v>
       </c>
@@ -674,8 +723,11 @@
       <c r="F10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>34</v>
       </c>
@@ -694,8 +746,11 @@
       <c r="F11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>34</v>
       </c>
@@ -709,13 +764,16 @@
         <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>34</v>
       </c>
@@ -734,8 +792,11 @@
       <c r="F13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>34</v>
       </c>
@@ -754,8 +815,11 @@
       <c r="F14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>34</v>
       </c>
@@ -774,8 +838,11 @@
       <c r="F15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>34</v>
       </c>
@@ -793,6 +860,9 @@
       </c>
       <c r="F16" t="s">
         <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Seed database with verified users and room equipment.
</commit_message>
<xml_diff>
--- a/RoomOccupancy.Persistence/Initializer/Files/SaleWzim.xlsx
+++ b/RoomOccupancy.Persistence/Initializer/Files/SaleWzim.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
   <si>
     <t xml:space="preserve"> Aula IV </t>
   </si>
@@ -52,28 +52,7 @@
     <t>Budynek</t>
   </si>
   <si>
-    <t>Wyposażenie</t>
-  </si>
-  <si>
-    <t>Projektor</t>
-  </si>
-  <si>
     <t>laboratorium komputerowe</t>
-  </si>
-  <si>
-    <t>Urządzenia sieciowe i budowa sieci, Projektor</t>
-  </si>
-  <si>
-    <t>Oscyloskop, Płytka badawcza układu scalonego</t>
-  </si>
-  <si>
-    <t>Projektor, Stanowiska komputerowe</t>
-  </si>
-  <si>
-    <t>Stanowiska komputerowe, Urządzenia sieciowe i budowa sieci, Projektor</t>
-  </si>
-  <si>
-    <t>Płytka badawcza układu scalonego, Oscyloskop</t>
   </si>
 </sst>
 </file>
@@ -483,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,10 +476,9 @@
     <col min="4" max="4" width="23.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -519,11 +497,8 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>34</v>
       </c>
@@ -542,11 +517,8 @@
       <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>34</v>
       </c>
@@ -565,11 +537,8 @@
       <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>34</v>
       </c>
@@ -589,7 +558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>34</v>
       </c>
@@ -608,11 +577,8 @@
       <c r="F5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>34</v>
       </c>
@@ -631,11 +597,8 @@
       <c r="F6" t="s">
         <v>2</v>
       </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>34</v>
       </c>
@@ -654,11 +617,8 @@
       <c r="F7" t="s">
         <v>2</v>
       </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>34</v>
       </c>
@@ -672,16 +632,13 @@
         <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
         <v>2</v>
       </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>34</v>
       </c>
@@ -700,11 +657,8 @@
       <c r="F9" t="s">
         <v>2</v>
       </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>34</v>
       </c>
@@ -723,11 +677,8 @@
       <c r="F10" t="s">
         <v>2</v>
       </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>34</v>
       </c>
@@ -746,11 +697,8 @@
       <c r="F11" t="s">
         <v>2</v>
       </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>34</v>
       </c>
@@ -764,16 +712,13 @@
         <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
         <v>2</v>
       </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>34</v>
       </c>
@@ -792,11 +737,8 @@
       <c r="F13" t="s">
         <v>2</v>
       </c>
-      <c r="G13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>34</v>
       </c>
@@ -815,11 +757,8 @@
       <c r="F14" t="s">
         <v>2</v>
       </c>
-      <c r="G14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>34</v>
       </c>
@@ -838,11 +777,8 @@
       <c r="F15" t="s">
         <v>2</v>
       </c>
-      <c r="G15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>34</v>
       </c>
@@ -860,9 +796,6 @@
       </c>
       <c r="F16" t="s">
         <v>2</v>
-      </c>
-      <c r="G16" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>